<commit_message>
actual change constratint excel
</commit_message>
<xml_diff>
--- a/baseSegment.xlsx
+++ b/baseSegment.xlsx
@@ -37,7 +37,7 @@
     <t>freestyle</t>
   </si>
   <si>
-    <t>Any</t>
+    <t>Same</t>
   </si>
   <si>
     <t>No drill</t>
@@ -46,7 +46,7 @@
     <t>No kick</t>
   </si>
   <si>
-    <t>Same</t>
+    <t>Any</t>
   </si>
   <si>
     <t>None</t>
@@ -59,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -71,13 +71,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,8 +101,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -109,6 +120,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -122,7 +155,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -131,7 +164,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -140,43 +173,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -185,28 +218,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -216,59 +264,65 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -288,8 +342,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -308,10 +364,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -488,11 +544,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -501,33 +560,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -766,12 +825,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1052,7 +1111,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1320,11 +1379,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -1336,294 +1393,294 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" ht="32.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="6">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="E2" t="s" s="6">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="F2" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" t="s" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>5</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="D3" t="s" s="10">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="8">
+      <c r="E3" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="F3" t="s" s="8">
+      <c r="F3" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="10">
+      <c r="A4" t="s" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="13">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="12">
+      <c r="C4" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="D4" t="s" s="12">
+      <c r="D4" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E4" t="s" s="12">
+      <c r="E4" t="s" s="14">
         <v>9</v>
       </c>
-      <c r="F4" t="s" s="12">
+      <c r="F4" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="16">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="14">
+      <c r="E5" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="C5" t="s" s="12">
+      <c r="D6" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="D5" t="s" s="12">
+      <c r="E6" t="s" s="14">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E5" t="s" s="12">
+      <c r="D7" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="F5" t="s" s="12">
+      <c r="E7" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s" s="16">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s" s="12">
+      <c r="E8" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s" s="12">
+      <c r="F8" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="D7" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s" s="12">
-        <v>10</v>
-      </c>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s" s="14">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s" s="12">
-        <v>8</v>
-      </c>
-      <c r="G8" s="13"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="13"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="13"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="13"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="13"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="13"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="13"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="13"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="13"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="13"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="13"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="13"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="13"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="13"/>
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="13"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="13"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>